<commit_message>
updated teamrankings ats, OU, wins scripts
</commit_message>
<xml_diff>
--- a/nba/teamrankings/team_stats/team_overall_stats/teams/minnesota-timberwolves/minnesota-timberwolves_stats.xlsx
+++ b/nba/teamrankings/team_stats/team_overall_stats/teams/minnesota-timberwolves/minnesota-timberwolves_stats.xlsx
@@ -473,7 +473,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>112.9 (#19)</t>
+          <t>113.1 (#18)</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -483,7 +483,7 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>109.0 (#6)</t>
+          <t>108.9 (#6)</t>
         </is>
       </c>
     </row>
@@ -500,7 +500,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>+3.8 (#8)</t>
+          <t>+4.2 (#8)</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -510,7 +510,7 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>-3.8 (#8)</t>
+          <t>-4.2 (#8)</t>
         </is>
       </c>
     </row>
@@ -527,7 +527,7 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>13.3 (#26)</t>
+          <t>13.4 (#26)</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -537,7 +537,7 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>14.3 (#6)</t>
+          <t>14.2 (#6)</t>
         </is>
       </c>
     </row>
@@ -554,7 +554,7 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>45.5 (#25)</t>
+          <t>45.9 (#22)</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -581,7 +581,7 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>25.8 (#17)</t>
+          <t>25.9 (#17)</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -591,7 +591,7 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>24.6 (#5)</t>
+          <t>24.4 (#4)</t>
         </is>
       </c>
     </row>
@@ -608,7 +608,7 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>52.0 (#17)</t>
+          <t>52.2 (#17)</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
@@ -618,7 +618,7 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>51.6 (#9)</t>
+          <t>51.4 (#7)</t>
         </is>
       </c>
     </row>
@@ -635,7 +635,7 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>0.640 (#13)</t>
+          <t>0.640 (#14)</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
@@ -645,7 +645,7 @@
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>0.609 (#4)</t>
+          <t>0.606 (#4)</t>
         </is>
       </c>
     </row>
@@ -662,7 +662,7 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>1.777 (#20)</t>
+          <t>1.787 (#20)</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
@@ -672,7 +672,7 @@
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>1.672 (#6)</t>
+          <t>1.658 (#6)</t>
         </is>
       </c>
     </row>
@@ -689,7 +689,7 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>54.9% (#11)</t>
+          <t>55.0% (#11)</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
@@ -699,7 +699,7 @@
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>53.0% (#6)</t>
+          <t>52.9% (#6)</t>
         </is>
       </c>
     </row>
@@ -716,7 +716,7 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>0.245 (#16)</t>
+          <t>0.247 (#13)</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
@@ -726,7 +726,7 @@
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>0.233 (#12)</t>
+          <t>0.232 (#11)</t>
         </is>
       </c>
     </row>
@@ -743,7 +743,7 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>79.5% (#7)</t>
+          <t>79.1% (#9)</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
@@ -753,7 +753,7 @@
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>77.2% (#8)</t>
+          <t>77.4% (#8)</t>
         </is>
       </c>
     </row>
@@ -770,7 +770,7 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>38.0% (#5)</t>
+          <t>37.9% (#5)</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
@@ -780,7 +780,7 @@
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>34.7% (#4)</t>
+          <t>34.8% (#3)</t>
         </is>
       </c>
     </row>
@@ -797,7 +797,7 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>53.2% (#22)</t>
+          <t>53.5% (#20)</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
@@ -807,7 +807,7 @@
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>53.6% (#10)</t>
+          <t>53.4% (#9)</t>
         </is>
       </c>
     </row>
@@ -824,7 +824,7 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>46.2% (#17)</t>
+          <t>46.4% (#17)</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
@@ -851,7 +851,7 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>1.158 (#11)</t>
+          <t>1.159 (#11)</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
@@ -878,7 +878,7 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>40.3 (#24)</t>
+          <t>40.5 (#22)</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
@@ -888,7 +888,7 @@
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>40.3 (#7)</t>
+          <t>40.3 (#5)</t>
         </is>
       </c>
     </row>
@@ -932,7 +932,7 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>15.2 (#5)</t>
+          <t>15.1 (#5)</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
@@ -959,7 +959,7 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>40.0 (#5)</t>
+          <t>39.9 (#5)</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
@@ -969,7 +969,7 @@
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>36.1 (#7)</t>
+          <t>36.0 (#6)</t>
         </is>
       </c>
     </row>
@@ -986,7 +986,7 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>17.0 (#16)</t>
+          <t>17.0 (#14)</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
@@ -996,7 +996,7 @@
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>15.8 (#6)</t>
+          <t>15.8 (#5)</t>
         </is>
       </c>
     </row>
@@ -1013,7 +1013,7 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>21.4 (#20)</t>
+          <t>21.5 (#19)</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
@@ -1023,7 +1023,7 @@
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>20.5 (#6)</t>
+          <t>20.4 (#5)</t>
         </is>
       </c>
     </row>
@@ -1040,7 +1040,7 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>28.0 (#18)</t>
+          <t>28.2 (#16)</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
@@ -1050,7 +1050,7 @@
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>27.7 (#11)</t>
+          <t>27.6 (#8)</t>
         </is>
       </c>
     </row>
@@ -1067,7 +1067,7 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>27.2 (#23)</t>
+          <t>27.3 (#24)</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
@@ -1077,7 +1077,7 @@
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>26.7 (#1)</t>
+          <t>26.8 (#2)</t>
         </is>
       </c>
     </row>
@@ -1094,7 +1094,7 @@
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>28.7 (#17)</t>
+          <t>28.7 (#19)</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
@@ -1121,7 +1121,7 @@
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>28.4 (#8)</t>
+          <t>28.6 (#7)</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
@@ -1148,7 +1148,7 @@
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>0.5 (#16)</t>
+          <t>0.5 (#15)</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
@@ -1185,7 +1185,7 @@
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>11.3 (#18)</t>
+          <t>11.2 (#16)</t>
         </is>
       </c>
     </row>
@@ -1202,7 +1202,7 @@
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>33.0 (#19)</t>
+          <t>33.1 (#18)</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
@@ -1212,7 +1212,7 @@
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>32.3 (#11)</t>
+          <t>32.3 (#10)</t>
         </is>
       </c>
     </row>
@@ -1229,17 +1229,17 @@
       </c>
       <c r="C30" t="inlineStr">
         <is>
+          <t>25.4% (#16)</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>Opp Off Rebound %</t>
+        </is>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
           <t>25.3% (#15)</t>
-        </is>
-      </c>
-      <c r="D30" t="inlineStr">
-        <is>
-          <t>Opp Off Rebound %</t>
-        </is>
-      </c>
-      <c r="E30" t="inlineStr">
-        <is>
-          <t>25.5% (#17)</t>
         </is>
       </c>
     </row>
@@ -1256,7 +1256,7 @@
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>74.5% (#17)</t>
+          <t>74.7% (#15)</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
@@ -1266,7 +1266,7 @@
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>74.7% (#15)</t>
+          <t>74.6% (#16)</t>
         </is>
       </c>
     </row>
@@ -1293,7 +1293,7 @@
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>4.7 (#12)</t>
+          <t>4.6 (#11)</t>
         </is>
       </c>
     </row>
@@ -1310,7 +1310,7 @@
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>5.5% (#16)</t>
+          <t>5.5% (#15)</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
@@ -1320,7 +1320,7 @@
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>5.4% (#14)</t>
+          <t>5.3% (#12)</t>
         </is>
       </c>
     </row>
@@ -1337,7 +1337,7 @@
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>8.1 (#15)</t>
+          <t>8.1 (#13)</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
@@ -1347,7 +1347,7 @@
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>8.6 (#20)</t>
+          <t>8.6 (#19)</t>
         </is>
       </c>
     </row>
@@ -1364,7 +1364,7 @@
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>7.2% (#12)</t>
+          <t>7.2% (#11)</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
@@ -1374,7 +1374,7 @@
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>7.7% (#22)</t>
+          <t>7.7% (#21)</t>
         </is>
       </c>
     </row>
@@ -1418,7 +1418,7 @@
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>13.0% (#20)</t>
+          <t>12.9% (#19)</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
@@ -1445,7 +1445,7 @@
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>18.1 (#9)</t>
+          <t>18.1 (#10)</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
@@ -1455,7 +1455,7 @@
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>18.9 (#12)</t>
+          <t>19.0 (#11)</t>
         </is>
       </c>
     </row>
@@ -1482,7 +1482,7 @@
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>0.3 (#12)</t>
+          <t>0.3 (#15)</t>
         </is>
       </c>
     </row>
@@ -1499,7 +1499,7 @@
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>16.1% (#14)</t>
+          <t>16.1% (#13)</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
@@ -1509,7 +1509,7 @@
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>16.9% (#9)</t>
+          <t>16.9% (#8)</t>
         </is>
       </c>
     </row>

</xml_diff>